<commit_message>
updates and pdf figures.
</commit_message>
<xml_diff>
--- a/data/raw/jho_temporal_data_summarized.xlsx
+++ b/data/raw/jho_temporal_data_summarized.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="35">
   <si>
     <t>year</t>
   </si>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,14 +1723,10 @@
     <col min="3" max="3" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1747,7 +1743,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1998</v>
       </c>
@@ -1764,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1998</v>
       </c>
@@ -1781,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1998</v>
       </c>
@@ -1798,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1998</v>
       </c>
@@ -1815,7 +1811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1998</v>
       </c>
@@ -1832,7 +1828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1998</v>
       </c>
@@ -1849,7 +1845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1998</v>
       </c>
@@ -1866,7 +1862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1998</v>
       </c>
@@ -1883,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1998</v>
       </c>
@@ -1899,9 +1895,8 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1998</v>
       </c>
@@ -1917,9 +1912,8 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1998</v>
       </c>
@@ -1935,9 +1929,8 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1998</v>
       </c>
@@ -1953,9 +1946,8 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2014</v>
       </c>
@@ -1971,9 +1963,8 @@
       <c r="E14" s="1">
         <v>10.666700000000001</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2014</v>
       </c>
@@ -1989,9 +1980,8 @@
       <c r="E15" s="1">
         <v>24</v>
       </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2014</v>
       </c>
@@ -2007,9 +1997,8 @@
       <c r="E16" s="1">
         <v>96</v>
       </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2014</v>
       </c>
@@ -2025,9 +2014,8 @@
       <c r="E17" s="1">
         <v>26.666699999999999</v>
       </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2014</v>
       </c>
@@ -2043,9 +2031,8 @@
       <c r="E18" s="1">
         <v>13.333299999999999</v>
       </c>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2014</v>
       </c>
@@ -2061,9 +2048,8 @@
       <c r="E19" s="1">
         <v>13.333299999999999</v>
       </c>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2014</v>
       </c>
@@ -2079,9 +2065,8 @@
       <c r="E20" s="1">
         <v>36</v>
       </c>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2014</v>
       </c>
@@ -2098,7 +2083,7 @@
         <v>37.333300000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2014</v>
       </c>
@@ -2115,7 +2100,7 @@
         <v>73.333299999999994</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2014</v>
       </c>
@@ -2132,7 +2117,7 @@
         <v>2.6667000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2014</v>
       </c>
@@ -2149,7 +2134,7 @@
         <v>1.3332999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2014</v>
       </c>
@@ -2166,7 +2151,7 @@
         <v>105.33329999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2014</v>
       </c>
@@ -2183,7 +2168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2014</v>
       </c>
@@ -2200,7 +2185,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2014</v>
       </c>
@@ -2217,7 +2202,7 @@
         <v>21.333300000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2014</v>
       </c>
@@ -2234,7 +2219,7 @@
         <v>1.3332999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2014</v>
       </c>
@@ -2251,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2014</v>
       </c>
@@ -2268,7 +2253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2014</v>
       </c>
@@ -4340,6 +4325,210 @@
       </c>
       <c r="E153" s="1">
         <v>19.45</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E154" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E155" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E157" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E158" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E159" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E160" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E161" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E162" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E163" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E164" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E165" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>